<commit_message>
Add check for blank value in DelimitedConverterImpl.generateLocalName to avoid instances with blank local names. Update tests to have an example of what should be a skipped object property value.
</commit_message>
<xml_diff>
--- a/com.mobi.etl.delimited/src/test/resources/testFileWithBlanks.xlsx
+++ b/com.mobi.etl.delimited/src/test/resources/testFileWithBlanks.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissa/gitrepos/matonto/org.matonto.etl.delimited/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganmercer/matonto/com.mobi.etl.delimited/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Source</t>
   </si>
@@ -413,7 +413,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -631,9 +631,6 @@
       </c>
       <c r="B11" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
       </c>
       <c r="D11" s="1">
         <v>3.0979999999999999</v>

</xml_diff>